<commit_message>
Performer ITM & SOZ angepasst
</commit_message>
<xml_diff>
--- a/Serienbrief_Performer_ITM/Data/Config.xlsx
+++ b/Serienbrief_Performer_ITM/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timotheus.vrettos\develop\develop_RPA\uipath-rpa_lob\Serienbrief_Performer_ITM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F235CCC-BAFF-4C9B-BAC9-0CD8AFDA344F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB81D78-9897-4C89-8D09-500B6C67C878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17445" yWindow="-12165" windowWidth="17280" windowHeight="8970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-50640" yWindow="-4260" windowWidth="38700" windowHeight="15375" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -244,9 +244,6 @@
     <t>rpa001_InputFolderPath</t>
   </si>
   <si>
-    <t>rpa001_inProgressFolderPath</t>
-  </si>
-  <si>
     <t>rpa001_FailedFolderPath</t>
   </si>
   <si>
@@ -293,6 +290,9 @@
   </si>
   <si>
     <t>rpa001_EmailSubjectLine</t>
+  </si>
+  <si>
+    <t>firefox, EXCEL, WINWORD</t>
   </si>
 </sst>
 </file>
@@ -723,7 +723,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -734,7 +734,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -748,7 +748,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -1758,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1841,6 +1841,9 @@
       <c r="A5" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="B5" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="C5" s="5" t="s">
         <v>46</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>66</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3020,10 +3023,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3128,18 +3131,18 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -3167,21 +3170,14 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>78</v>
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" t="s">
-        <v>83</v>
-      </c>
-    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -4165,7 +4161,6 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>